<commit_message>
optimize rule template file
</commit_message>
<xml_diff>
--- a/shardingsphere-ui-backend/src/main/resources/template/系统敏感信息采集表模板.xlsx
+++ b/shardingsphere-ui-backend/src/main/resources/template/系统敏感信息采集表模板.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9420"/>
+    <workbookView windowWidth="19200" windowHeight="7130"/>
   </bookViews>
   <sheets>
     <sheet name="数据库敏感信息采集表" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,34 @@
     <author>Administrator</author>
   </authors>
   <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>mysql数据库忽略该字段
+postgresql请填写该字段</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>用于对历史数据加密过程中表存在增量数据
+否：不是增量字段
+是：增量字段
+若一个表定义多个增量字段则取只其中一个</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G1" authorId="0">
       <text>
         <r>
@@ -31,7 +59,8 @@
             <charset val="134"/>
           </rPr>
           <t>对称加密：AES,SM4,RC4
-非对称：MD5,SM3</t>
+非对称：MD5,SM3
+注：若为增量字段，无需定义该值，若定义，则忽略</t>
         </r>
       </text>
     </comment>
@@ -43,7 +72,11 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t>针对对称加密定义密钥</t>
+          <t xml:space="preserve">针对对称加密定义密钥
+对称加密：AES,SM4,RC4
+非对称：MD5,SM3
+注：若为增量字段，无需定义该值，若定义，则忽略
+</t>
         </r>
       </text>
     </comment>
@@ -52,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>数据库名称</t>
   </si>
@@ -88,6 +121,21 @@
   </si>
   <si>
     <t>varchar</t>
+  </si>
+  <si>
+    <t>AES</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>update_time</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>是</t>
   </si>
 </sst>
 </file>
@@ -95,10 +143,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -116,28 +164,58 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -147,14 +225,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -162,33 +233,17 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -231,6 +286,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -241,20 +303,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -274,55 +322,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,121 +496,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,6 +513,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -490,30 +562,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -573,10 +621,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -585,133 +633,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1044,22 +1092,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="21.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="21.775" customWidth="1"/>
     <col min="2" max="2" width="12.4166666666667" customWidth="1"/>
-    <col min="3" max="3" width="40.7777777777778" customWidth="1"/>
+    <col min="3" max="3" width="40.775" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="16.1666666666667" customWidth="1"/>
-    <col min="6" max="6" width="32.2222222222222" customWidth="1"/>
+    <col min="6" max="6" width="32.225" customWidth="1"/>
     <col min="7" max="7" width="20.4166666666667" style="1" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
@@ -1090,7 +1138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1102,6 +1150,29 @@
       </c>
       <c r="E2" t="s">
         <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat:模板加标注-区分大小写 optimize file import
</commit_message>
<xml_diff>
--- a/shardingsphere-ui-backend/src/main/resources/template/系统敏感信息采集表模板.xlsx
+++ b/shardingsphere-ui-backend/src/main/resources/template/系统敏感信息采集表模板.xlsx
@@ -22,6 +22,18 @@
     <author>Administrator</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>注：区分大小写</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B1" authorId="0">
       <text>
         <r>
@@ -31,7 +43,34 @@
             <charset val="134"/>
           </rPr>
           <t>mysql数据库忽略该字段
-postgresql请填写该字段</t>
+postgresql请填写该字段
+注：区分大小写</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">注：区分大小写
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">注：区分大小写
+</t>
         </r>
       </text>
     </comment>
@@ -143,10 +182,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -165,6 +204,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -178,70 +232,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -262,14 +294,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -278,31 +302,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -322,37 +361,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,145 +535,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,6 +552,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -535,7 +598,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -551,41 +614,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,11 +638,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -621,10 +660,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -633,133 +672,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1097,7 +1136,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="7"/>

</xml_diff>